<commit_message>
Atualizada documentação para landPage e recolocação de dados de categoria
</commit_message>
<xml_diff>
--- a/Documentação/Documentação.xlsx
+++ b/Documentação/Documentação.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\25203678\Projeto_integrador\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38352743-C688-42D6-845D-BE17014EE5B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C820F2-CC33-4BC4-9E47-8379C9D20AF2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6810" xr2:uid="{0C2E8A2F-6BFD-4C92-8FD1-094373D586EB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6810" xr2:uid="{0C2E8A2F-6BFD-4C92-8FD1-094373D586EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
   <si>
     <t>Organização</t>
   </si>
@@ -78,12 +78,6 @@
     <t>Categoria</t>
   </si>
   <si>
-    <t>RNF01</t>
-  </si>
-  <si>
-    <t>RNF02</t>
-  </si>
-  <si>
     <t>Requisitos de negócio</t>
   </si>
   <si>
@@ -144,15 +138,9 @@
     <t>RNF 02 - A aplicação deve ser codificado em linguagem de programação JAVA e JAVAFX.</t>
   </si>
   <si>
-    <t>RNF03</t>
-  </si>
-  <si>
     <t>RNF 03 - A aplicação deve localizar o registro de veículos em arquivo CSV, por placa, em “Veículos estacionados”.</t>
   </si>
   <si>
-    <t>RNF04</t>
-  </si>
-  <si>
     <t>RNF 04 - A aplicação deve exibir uma lista (TableView) com veículos estacionados.</t>
   </si>
   <si>
@@ -163,13 +151,70 @@
   </si>
   <si>
     <t>RN 03 - A aplicação deve ser de total autoria da empresa, podendo entregar as solicitações de clientes apenas as licenças.</t>
+  </si>
+  <si>
+    <t>RF10 - A llanding page deve ter botões que possibilitam informação clara e rápida</t>
+  </si>
+  <si>
+    <t>RF11 - A landing page deve possuir método de clientes</t>
+  </si>
+  <si>
+    <t>RF12 - A landing page deve ter método de planos, anual e mensal</t>
+  </si>
+  <si>
+    <t>RF13 - A landing page deve ter formulário para agendar consulta</t>
+  </si>
+  <si>
+    <t>RF15 - A landing page deve ter área de cabeçalho para movimentação rápida</t>
+  </si>
+  <si>
+    <t>RF16 - A landing page deve ter imagem e área de demonstração da aplicação web</t>
+  </si>
+  <si>
+    <t>RF09 - A landing page, deve ser de fácil entendimento, com coloração chamativa</t>
+  </si>
+  <si>
+    <t>RF14 - A landing page deve ter área que mostra contatos</t>
+  </si>
+  <si>
+    <t>RF16 - A landing page deve ter imagem de fundo de estacionamento</t>
+  </si>
+  <si>
+    <t>RF17 - A landing page deve ter  método chamativo para segurança, e confiabilidade</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">      </t>
+  </si>
+  <si>
+    <t>RNF01 -</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RNF02 - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desempenho (velocidade, capacidade), Segurança (proteção de dados), Usabilidade (facilidade de uso), Disponibilidade (uptime), Confiabilidade (backup, integridade), Escalabilidade, Portabilidade (compatibilidade com navegadores/SO), Interoperabilidade (integração com outros sistemas) e Manutenibilidade. </t>
+  </si>
+  <si>
+    <t>Usabilidade</t>
+  </si>
+  <si>
+    <t>Usabilidade e portabilidade</t>
+  </si>
+  <si>
+    <t>RNF03 -</t>
+  </si>
+  <si>
+    <t>RNF04 -</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,6 +284,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -704,7 +755,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -757,12 +808,256 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -772,249 +1067,18 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1331,10 +1395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91C1A38B-CAB9-46D2-BE9F-9CE279C13D95}">
-  <dimension ref="A1:L87"/>
+  <dimension ref="A1:L90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1344,18 +1408,19 @@
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="41.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="67.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="13"/>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="34"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="69"/>
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
@@ -1366,48 +1431,48 @@
       <c r="A2" s="1"/>
       <c r="B2" s="13"/>
       <c r="C2" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D2" s="14"/>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="37" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="38"/>
+      <c r="F2" s="72" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="73"/>
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
     </row>
-    <row r="3" spans="1:12" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="13"/>
       <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="14"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="40"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="75"/>
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
     </row>
-    <row r="4" spans="1:12" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="13"/>
       <c r="C4" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D4" s="14"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="40"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="75"/>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
       <c r="J4" s="12"/>
@@ -1418,12 +1483,12 @@
       <c r="A5" s="1"/>
       <c r="B5" s="13"/>
       <c r="C5" s="16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D5" s="14"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="42"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="77"/>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
@@ -1433,15 +1498,15 @@
     <row r="6" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="13"/>
-      <c r="C6" s="50">
+      <c r="C6" s="18">
         <v>45987</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="43"/>
-      <c r="G6" s="44"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="79"/>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -1465,13 +1530,13 @@
     <row r="8" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="13"/>
-      <c r="C8" s="45" t="s">
+      <c r="C8" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="47"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="81"/>
+      <c r="G8" s="82"/>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
@@ -1484,10 +1549,10 @@
       <c r="C9" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="48" t="s">
+      <c r="D9" s="83" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="49"/>
+      <c r="E9" s="84"/>
       <c r="F9" s="6" t="s">
         <v>7</v>
       </c>
@@ -1503,18 +1568,18 @@
     <row r="10" spans="1:12" ht="105.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="13"/>
-      <c r="C10" s="51" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="52" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="52"/>
-      <c r="F10" s="53">
+      <c r="C10" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="20"/>
+      <c r="F10" s="21">
         <v>45987</v>
       </c>
-      <c r="G10" s="54" t="s">
-        <v>26</v>
+      <c r="G10" s="22" t="s">
+        <v>24</v>
       </c>
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
@@ -1861,13 +1926,13 @@
     <row r="35" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="12"/>
-      <c r="C35" s="23" t="s">
+      <c r="C35" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
+      <c r="D35" s="85"/>
+      <c r="E35" s="85"/>
+      <c r="F35" s="85"/>
+      <c r="G35" s="85"/>
       <c r="H35" s="12"/>
       <c r="I35" s="12"/>
       <c r="J35" s="12"/>
@@ -1893,13 +1958,13 @@
     <row r="37" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="13"/>
-      <c r="C37" s="55" t="s">
-        <v>25</v>
-      </c>
-      <c r="D37" s="56"/>
-      <c r="E37" s="56"/>
-      <c r="F37" s="56"/>
-      <c r="G37" s="57"/>
+      <c r="C37" s="86" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37" s="87"/>
+      <c r="E37" s="87"/>
+      <c r="F37" s="87"/>
+      <c r="G37" s="88"/>
       <c r="H37" s="12"/>
       <c r="I37" s="12"/>
       <c r="J37" s="12"/>
@@ -1909,11 +1974,11 @@
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="13"/>
-      <c r="C38" s="58"/>
-      <c r="D38" s="59"/>
-      <c r="E38" s="59"/>
-      <c r="F38" s="59"/>
-      <c r="G38" s="60"/>
+      <c r="C38" s="89"/>
+      <c r="D38" s="90"/>
+      <c r="E38" s="90"/>
+      <c r="F38" s="90"/>
+      <c r="G38" s="91"/>
       <c r="H38" s="12"/>
       <c r="I38" s="12"/>
       <c r="J38" s="12"/>
@@ -1923,11 +1988,11 @@
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="13"/>
-      <c r="C39" s="58"/>
-      <c r="D39" s="59"/>
-      <c r="E39" s="59"/>
-      <c r="F39" s="59"/>
-      <c r="G39" s="60"/>
+      <c r="C39" s="89"/>
+      <c r="D39" s="90"/>
+      <c r="E39" s="90"/>
+      <c r="F39" s="90"/>
+      <c r="G39" s="91"/>
       <c r="H39" s="12"/>
       <c r="I39" s="12"/>
       <c r="J39" s="12"/>
@@ -1937,11 +2002,11 @@
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="13"/>
-      <c r="C40" s="58"/>
-      <c r="D40" s="59"/>
-      <c r="E40" s="59"/>
-      <c r="F40" s="59"/>
-      <c r="G40" s="60"/>
+      <c r="C40" s="89"/>
+      <c r="D40" s="90"/>
+      <c r="E40" s="90"/>
+      <c r="F40" s="90"/>
+      <c r="G40" s="91"/>
       <c r="H40" s="12"/>
       <c r="I40" s="12"/>
       <c r="J40" s="12"/>
@@ -1951,12 +2016,12 @@
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="13"/>
-      <c r="C41" s="58"/>
-      <c r="D41" s="59"/>
-      <c r="E41" s="59"/>
-      <c r="F41" s="59"/>
-      <c r="G41" s="60"/>
-      <c r="H41" s="104"/>
+      <c r="C41" s="89"/>
+      <c r="D41" s="90"/>
+      <c r="E41" s="90"/>
+      <c r="F41" s="90"/>
+      <c r="G41" s="91"/>
+      <c r="H41" s="47"/>
       <c r="I41" s="12"/>
       <c r="J41" s="12"/>
       <c r="K41" s="12"/>
@@ -1965,11 +2030,11 @@
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="13"/>
-      <c r="C42" s="58"/>
-      <c r="D42" s="59"/>
-      <c r="E42" s="59"/>
-      <c r="F42" s="59"/>
-      <c r="G42" s="60"/>
+      <c r="C42" s="89"/>
+      <c r="D42" s="90"/>
+      <c r="E42" s="90"/>
+      <c r="F42" s="90"/>
+      <c r="G42" s="91"/>
       <c r="H42" s="12"/>
       <c r="I42" s="12"/>
       <c r="J42" s="12"/>
@@ -1979,11 +2044,11 @@
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="13"/>
-      <c r="C43" s="58"/>
-      <c r="D43" s="59"/>
-      <c r="E43" s="59"/>
-      <c r="F43" s="59"/>
-      <c r="G43" s="60"/>
+      <c r="C43" s="89"/>
+      <c r="D43" s="90"/>
+      <c r="E43" s="90"/>
+      <c r="F43" s="90"/>
+      <c r="G43" s="91"/>
       <c r="H43" s="12"/>
       <c r="I43" s="12"/>
       <c r="J43" s="12"/>
@@ -1993,11 +2058,11 @@
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="13"/>
-      <c r="C44" s="58"/>
-      <c r="D44" s="59"/>
-      <c r="E44" s="59"/>
-      <c r="F44" s="59"/>
-      <c r="G44" s="60"/>
+      <c r="C44" s="89"/>
+      <c r="D44" s="90"/>
+      <c r="E44" s="90"/>
+      <c r="F44" s="90"/>
+      <c r="G44" s="91"/>
       <c r="H44" s="12"/>
       <c r="I44" s="12"/>
       <c r="J44" s="12"/>
@@ -2007,11 +2072,11 @@
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="13"/>
-      <c r="C45" s="58"/>
-      <c r="D45" s="59"/>
-      <c r="E45" s="59"/>
-      <c r="F45" s="59"/>
-      <c r="G45" s="60"/>
+      <c r="C45" s="89"/>
+      <c r="D45" s="90"/>
+      <c r="E45" s="90"/>
+      <c r="F45" s="90"/>
+      <c r="G45" s="91"/>
       <c r="H45" s="12"/>
       <c r="I45" s="12"/>
       <c r="J45" s="12"/>
@@ -2021,11 +2086,11 @@
     <row r="46" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="13"/>
-      <c r="C46" s="61"/>
-      <c r="D46" s="62"/>
-      <c r="E46" s="62"/>
-      <c r="F46" s="62"/>
-      <c r="G46" s="63"/>
+      <c r="C46" s="92"/>
+      <c r="D46" s="93"/>
+      <c r="E46" s="93"/>
+      <c r="F46" s="93"/>
+      <c r="G46" s="94"/>
       <c r="H46" s="12"/>
       <c r="I46" s="12"/>
       <c r="J46" s="12"/>
@@ -2049,13 +2114,13 @@
     <row r="48" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="13"/>
-      <c r="C48" s="24" t="s">
+      <c r="C48" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="D48" s="25"/>
-      <c r="E48" s="25"/>
-      <c r="F48" s="25"/>
-      <c r="G48" s="26"/>
+      <c r="D48" s="95"/>
+      <c r="E48" s="95"/>
+      <c r="F48" s="95"/>
+      <c r="G48" s="96"/>
       <c r="H48" s="12"/>
       <c r="I48" s="12"/>
       <c r="J48" s="12"/>
@@ -2065,13 +2130,13 @@
     <row r="49" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="13"/>
-      <c r="C49" s="27" t="s">
+      <c r="C49" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="D49" s="28"/>
-      <c r="E49" s="28"/>
-      <c r="F49" s="28"/>
-      <c r="G49" s="29"/>
+      <c r="D49" s="98"/>
+      <c r="E49" s="98"/>
+      <c r="F49" s="98"/>
+      <c r="G49" s="99"/>
       <c r="H49" s="12"/>
       <c r="I49" s="12"/>
       <c r="J49" s="12"/>
@@ -2084,142 +2149,142 @@
       <c r="C50" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D50" s="64" t="s">
+      <c r="D50" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="E50" s="31"/>
-      <c r="F50" s="30" t="s">
+      <c r="E50" s="100"/>
+      <c r="F50" s="101" t="s">
         <v>14</v>
       </c>
-      <c r="G50" s="65"/>
+      <c r="G50" s="62"/>
       <c r="H50" s="12"/>
       <c r="I50" s="12"/>
       <c r="J50" s="12"/>
       <c r="K50" s="12"/>
       <c r="L50" s="12"/>
     </row>
-    <row r="51" spans="1:12" ht="234" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" ht="18" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="13"/>
-      <c r="C51" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="D51" s="67"/>
-      <c r="E51" s="68"/>
-      <c r="F51" s="69"/>
-      <c r="G51" s="70"/>
+      <c r="C51" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D51" s="26"/>
+      <c r="E51" s="27"/>
+      <c r="F51" s="63"/>
+      <c r="G51" s="64"/>
       <c r="H51" s="12"/>
       <c r="I51" s="12"/>
       <c r="J51" s="12"/>
       <c r="K51" s="12"/>
       <c r="L51" s="12"/>
     </row>
-    <row r="52" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" ht="36" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="13"/>
-      <c r="C52" s="71" t="s">
-        <v>30</v>
-      </c>
-      <c r="D52" s="72"/>
+      <c r="C52" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="D52" s="29"/>
       <c r="E52" s="9"/>
-      <c r="F52" s="73"/>
-      <c r="G52" s="74"/>
+      <c r="F52" s="65"/>
+      <c r="G52" s="66"/>
       <c r="H52" s="12"/>
       <c r="I52" s="12"/>
       <c r="J52" s="12"/>
       <c r="K52" s="12"/>
       <c r="L52" s="12"/>
     </row>
-    <row r="53" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" ht="36" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="13"/>
-      <c r="C53" s="66" t="s">
-        <v>31</v>
-      </c>
-      <c r="D53" s="75"/>
-      <c r="E53" s="76"/>
-      <c r="F53" s="64"/>
-      <c r="G53" s="65"/>
+      <c r="C53" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="D53" s="30"/>
+      <c r="E53" s="31"/>
+      <c r="F53" s="61"/>
+      <c r="G53" s="62"/>
       <c r="H53" s="12"/>
       <c r="I53" s="12"/>
       <c r="J53" s="12"/>
       <c r="K53" s="12"/>
       <c r="L53" s="12"/>
     </row>
-    <row r="54" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" ht="36" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="13"/>
-      <c r="C54" s="77" t="s">
-        <v>32</v>
-      </c>
-      <c r="D54" s="75"/>
-      <c r="E54" s="76"/>
-      <c r="F54" s="64"/>
-      <c r="G54" s="65"/>
+      <c r="C54" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D54" s="30"/>
+      <c r="E54" s="31"/>
+      <c r="F54" s="61"/>
+      <c r="G54" s="62"/>
       <c r="H54" s="12"/>
       <c r="I54" s="12"/>
       <c r="J54" s="12"/>
       <c r="K54" s="12"/>
       <c r="L54" s="12"/>
     </row>
-    <row r="55" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" ht="18" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="13"/>
-      <c r="C55" s="77" t="s">
-        <v>33</v>
-      </c>
-      <c r="D55" s="75"/>
-      <c r="E55" s="76"/>
-      <c r="F55" s="64"/>
-      <c r="G55" s="65"/>
+      <c r="C55" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="D55" s="30"/>
+      <c r="E55" s="31"/>
+      <c r="F55" s="61"/>
+      <c r="G55" s="62"/>
       <c r="H55" s="12"/>
       <c r="I55" s="12"/>
       <c r="J55" s="12"/>
       <c r="K55" s="12"/>
       <c r="L55" s="12"/>
     </row>
-    <row r="56" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" ht="18" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="13"/>
-      <c r="C56" s="77" t="s">
-        <v>34</v>
-      </c>
-      <c r="D56" s="75"/>
-      <c r="E56" s="76"/>
-      <c r="F56" s="64"/>
-      <c r="G56" s="65"/>
+      <c r="C56" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="D56" s="30"/>
+      <c r="E56" s="31"/>
+      <c r="F56" s="61"/>
+      <c r="G56" s="62"/>
       <c r="H56" s="12"/>
       <c r="I56" s="12"/>
       <c r="J56" s="12"/>
       <c r="K56" s="12"/>
       <c r="L56" s="12"/>
     </row>
-    <row r="57" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" ht="36" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="13"/>
-      <c r="C57" s="77" t="s">
-        <v>35</v>
-      </c>
-      <c r="D57" s="75"/>
-      <c r="E57" s="76"/>
-      <c r="F57" s="64"/>
-      <c r="G57" s="65"/>
+      <c r="C57" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="D57" s="30"/>
+      <c r="E57" s="31"/>
+      <c r="F57" s="61"/>
+      <c r="G57" s="62"/>
       <c r="H57" s="12"/>
       <c r="I57" s="12"/>
       <c r="J57" s="12"/>
       <c r="K57" s="12"/>
       <c r="L57" s="12"/>
     </row>
-    <row r="58" spans="1:12" ht="288" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" ht="18" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="13"/>
-      <c r="C58" s="77" t="s">
-        <v>36</v>
-      </c>
-      <c r="D58" s="75"/>
-      <c r="E58" s="76"/>
-      <c r="F58" s="64"/>
-      <c r="G58" s="65"/>
+      <c r="C58" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="D58" s="30"/>
+      <c r="E58" s="31"/>
+      <c r="F58" s="61"/>
+      <c r="G58" s="62"/>
       <c r="H58" s="12"/>
       <c r="I58" s="12"/>
       <c r="J58" s="12"/>
@@ -2229,11 +2294,13 @@
     <row r="59" spans="1:12" ht="18" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="13"/>
-      <c r="C59" s="77"/>
-      <c r="D59" s="75"/>
-      <c r="E59" s="76"/>
-      <c r="F59" s="64"/>
-      <c r="G59" s="65"/>
+      <c r="C59" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="D59" s="30"/>
+      <c r="E59" s="31"/>
+      <c r="F59" s="61"/>
+      <c r="G59" s="62"/>
       <c r="H59" s="12"/>
       <c r="I59" s="12"/>
       <c r="J59" s="12"/>
@@ -2243,11 +2310,13 @@
     <row r="60" spans="1:12" ht="18" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="13"/>
-      <c r="C60" s="77"/>
-      <c r="D60" s="75"/>
-      <c r="E60" s="76"/>
-      <c r="F60" s="64"/>
-      <c r="G60" s="65"/>
+      <c r="C60" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="D60" s="30"/>
+      <c r="E60" s="31"/>
+      <c r="F60" s="61"/>
+      <c r="G60" s="62"/>
       <c r="H60" s="12"/>
       <c r="I60" s="12"/>
       <c r="J60" s="12"/>
@@ -2257,11 +2326,13 @@
     <row r="61" spans="1:12" ht="18" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="13"/>
-      <c r="C61" s="77"/>
-      <c r="D61" s="75"/>
-      <c r="E61" s="76"/>
-      <c r="F61" s="64"/>
-      <c r="G61" s="65"/>
+      <c r="C61" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="D61" s="30"/>
+      <c r="E61" s="31"/>
+      <c r="F61" s="61"/>
+      <c r="G61" s="62"/>
       <c r="H61" s="12"/>
       <c r="I61" s="12"/>
       <c r="J61" s="12"/>
@@ -2271,11 +2342,13 @@
     <row r="62" spans="1:12" ht="18" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="13"/>
-      <c r="C62" s="77"/>
-      <c r="D62" s="75"/>
-      <c r="E62" s="76"/>
-      <c r="F62" s="64"/>
-      <c r="G62" s="65"/>
+      <c r="C62" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="D62" s="30"/>
+      <c r="E62" s="31"/>
+      <c r="F62" s="61"/>
+      <c r="G62" s="62"/>
       <c r="H62" s="12"/>
       <c r="I62" s="12"/>
       <c r="J62" s="12"/>
@@ -2285,11 +2358,13 @@
     <row r="63" spans="1:12" ht="18" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="13"/>
-      <c r="C63" s="77"/>
-      <c r="D63" s="75"/>
-      <c r="E63" s="76"/>
-      <c r="F63" s="64"/>
-      <c r="G63" s="65"/>
+      <c r="C63" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="D63" s="30"/>
+      <c r="E63" s="31"/>
+      <c r="F63" s="61"/>
+      <c r="G63" s="62"/>
       <c r="H63" s="12"/>
       <c r="I63" s="12"/>
       <c r="J63" s="12"/>
@@ -2299,53 +2374,61 @@
     <row r="64" spans="1:12" ht="18" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="13"/>
-      <c r="C64" s="77"/>
-      <c r="D64" s="75"/>
-      <c r="E64" s="76"/>
-      <c r="F64" s="64"/>
-      <c r="G64" s="65"/>
+      <c r="C64" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="D64" s="30"/>
+      <c r="E64" s="31"/>
+      <c r="F64" s="61"/>
+      <c r="G64" s="62"/>
       <c r="H64" s="12"/>
-      <c r="I64" s="12"/>
+      <c r="I64" s="107"/>
       <c r="J64" s="12"/>
       <c r="K64" s="12"/>
       <c r="L64" s="12"/>
     </row>
-    <row r="65" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="1"/>
+    <row r="65" spans="1:12" ht="18" x14ac:dyDescent="0.25">
+      <c r="A65" s="13"/>
       <c r="B65" s="13"/>
-      <c r="C65" s="78"/>
-      <c r="D65" s="79"/>
-      <c r="E65" s="8"/>
-      <c r="F65" s="64"/>
-      <c r="G65" s="65"/>
+      <c r="C65" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="D65" s="30"/>
+      <c r="E65" s="31"/>
+      <c r="F65" s="23"/>
+      <c r="G65" s="24"/>
       <c r="H65" s="12"/>
       <c r="I65" s="12"/>
       <c r="J65" s="12"/>
       <c r="K65" s="12"/>
       <c r="L65" s="12"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A66" s="2"/>
-      <c r="B66" s="12"/>
-      <c r="C66" s="12"/>
-      <c r="D66" s="12"/>
-      <c r="E66" s="12"/>
-      <c r="F66" s="12"/>
-      <c r="G66" s="12"/>
+    <row r="66" spans="1:12" ht="18" x14ac:dyDescent="0.25">
+      <c r="A66" s="13"/>
+      <c r="B66" s="13"/>
+      <c r="C66" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D66" s="30"/>
+      <c r="E66" s="31"/>
+      <c r="F66" s="23"/>
+      <c r="G66" s="24"/>
       <c r="H66" s="12"/>
       <c r="I66" s="12"/>
       <c r="J66" s="12"/>
       <c r="K66" s="12"/>
       <c r="L66" s="12"/>
     </row>
-    <row r="67" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="2"/>
-      <c r="B67" s="12"/>
-      <c r="C67" s="10"/>
-      <c r="D67" s="10"/>
-      <c r="E67" s="10"/>
-      <c r="F67" s="10"/>
-      <c r="G67" s="10"/>
+    <row r="67" spans="1:12" ht="18" x14ac:dyDescent="0.25">
+      <c r="A67" s="13"/>
+      <c r="B67" s="13"/>
+      <c r="C67" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="D67" s="30"/>
+      <c r="E67" s="31"/>
+      <c r="F67" s="23"/>
+      <c r="G67" s="24"/>
       <c r="H67" s="12"/>
       <c r="I67" s="12"/>
       <c r="J67" s="12"/>
@@ -2353,205 +2436,221 @@
       <c r="L67" s="12"/>
     </row>
     <row r="68" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="11"/>
-      <c r="B68" s="11"/>
-      <c r="C68" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D68" s="21"/>
-      <c r="E68" s="21"/>
-      <c r="F68" s="21"/>
-      <c r="G68" s="22"/>
+      <c r="A68" s="1"/>
+      <c r="B68" s="13"/>
+      <c r="C68" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="D68" s="34"/>
+      <c r="E68" s="8"/>
+      <c r="F68" s="61"/>
+      <c r="G68" s="62"/>
       <c r="H68" s="12"/>
       <c r="I68" s="12"/>
       <c r="J68" s="12"/>
       <c r="K68" s="12"/>
       <c r="L68" s="12"/>
     </row>
-    <row r="69" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="11"/>
-      <c r="B69" s="11"/>
-      <c r="C69" s="80" t="s">
-        <v>13</v>
-      </c>
-      <c r="D69" s="81" t="s">
-        <v>16</v>
-      </c>
-      <c r="E69" s="82"/>
-      <c r="F69" s="81" t="s">
-        <v>8</v>
-      </c>
-      <c r="G69" s="82"/>
+    <row r="69" spans="1:12" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="2"/>
+      <c r="B69" s="12"/>
+      <c r="C69" s="109" t="s">
+        <v>56</v>
+      </c>
+      <c r="D69" s="108"/>
+      <c r="E69" s="108"/>
+      <c r="F69" s="108"/>
+      <c r="G69" s="108"/>
       <c r="H69" s="12"/>
       <c r="I69" s="12"/>
       <c r="J69" s="12"/>
       <c r="K69" s="12"/>
       <c r="L69" s="12"/>
     </row>
-    <row r="70" spans="1:12" ht="62.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="11"/>
-      <c r="B70" s="11"/>
-      <c r="C70" s="83" t="s">
-        <v>17</v>
-      </c>
-      <c r="D70" s="84"/>
-      <c r="E70" s="85"/>
-      <c r="F70" s="86" t="s">
-        <v>37</v>
-      </c>
-      <c r="G70" s="87"/>
+    <row r="70" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="2"/>
+      <c r="B70" s="12"/>
+      <c r="C70" s="10"/>
+      <c r="D70" s="10"/>
+      <c r="E70" s="10"/>
+      <c r="F70" s="10"/>
+      <c r="G70" s="10"/>
       <c r="H70" s="12"/>
       <c r="I70" s="12"/>
       <c r="J70" s="12"/>
       <c r="K70" s="12"/>
       <c r="L70" s="12"/>
     </row>
-    <row r="71" spans="1:12" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="11"/>
       <c r="B71" s="11"/>
-      <c r="C71" s="88" t="s">
-        <v>18</v>
-      </c>
-      <c r="D71" s="84"/>
-      <c r="E71" s="85"/>
-      <c r="F71" s="84" t="s">
-        <v>38</v>
-      </c>
-      <c r="G71" s="85"/>
+      <c r="C71" s="102" t="s">
+        <v>15</v>
+      </c>
+      <c r="D71" s="103"/>
+      <c r="E71" s="103"/>
+      <c r="F71" s="103"/>
+      <c r="G71" s="104"/>
       <c r="H71" s="12"/>
       <c r="I71" s="12"/>
       <c r="J71" s="12"/>
       <c r="K71" s="12"/>
       <c r="L71" s="12"/>
     </row>
-    <row r="72" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="2"/>
-      <c r="B72" s="12"/>
-      <c r="C72" s="89" t="s">
-        <v>39</v>
-      </c>
-      <c r="D72" s="90"/>
-      <c r="E72" s="85"/>
-      <c r="F72" s="84" t="s">
-        <v>40</v>
-      </c>
-      <c r="G72" s="85"/>
+    <row r="72" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="11"/>
+      <c r="B72" s="11"/>
+      <c r="C72" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="D72" s="59" t="s">
+        <v>16</v>
+      </c>
+      <c r="E72" s="58"/>
+      <c r="F72" s="59" t="s">
+        <v>8</v>
+      </c>
+      <c r="G72" s="58"/>
       <c r="H72" s="12"/>
       <c r="I72" s="12"/>
       <c r="J72" s="12"/>
       <c r="K72" s="12"/>
       <c r="L72" s="12"/>
     </row>
-    <row r="73" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="1"/>
-      <c r="B73" s="91"/>
-      <c r="C73" s="92" t="s">
-        <v>41</v>
-      </c>
-      <c r="D73" s="90"/>
-      <c r="E73" s="85"/>
-      <c r="F73" s="84" t="s">
-        <v>42</v>
-      </c>
-      <c r="G73" s="85"/>
+    <row r="73" spans="1:12" ht="62.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="11"/>
+      <c r="B73" s="11"/>
+      <c r="C73" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="D73" s="60" t="s">
+        <v>58</v>
+      </c>
+      <c r="E73" s="49"/>
+      <c r="F73" s="105" t="s">
+        <v>35</v>
+      </c>
+      <c r="G73" s="106"/>
       <c r="H73" s="12"/>
       <c r="I73" s="12"/>
       <c r="J73" s="12"/>
       <c r="K73" s="12"/>
       <c r="L73" s="12"/>
     </row>
-    <row r="74" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="11"/>
-      <c r="B74" s="91"/>
-      <c r="C74" s="92"/>
-      <c r="D74" s="90"/>
-      <c r="E74" s="85"/>
-      <c r="F74" s="84"/>
-      <c r="G74" s="85"/>
+      <c r="B74" s="11"/>
+      <c r="C74" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="D74" s="60" t="s">
+        <v>57</v>
+      </c>
+      <c r="E74" s="49"/>
+      <c r="F74" s="60" t="s">
+        <v>36</v>
+      </c>
+      <c r="G74" s="49"/>
       <c r="H74" s="12"/>
       <c r="I74" s="12"/>
       <c r="J74" s="12"/>
       <c r="K74" s="12"/>
       <c r="L74" s="12"/>
     </row>
-    <row r="75" spans="1:12" ht="62.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="11"/>
-      <c r="B75" s="91"/>
-      <c r="C75" s="93"/>
-      <c r="D75" s="90"/>
-      <c r="E75" s="85"/>
-      <c r="F75" s="84"/>
-      <c r="G75" s="85"/>
+    <row r="75" spans="1:12" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="2"/>
+      <c r="B75" s="12"/>
+      <c r="C75" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="D75" s="48" t="s">
+        <v>57</v>
+      </c>
+      <c r="E75" s="49"/>
+      <c r="F75" s="60" t="s">
+        <v>37</v>
+      </c>
+      <c r="G75" s="49"/>
       <c r="H75" s="12"/>
       <c r="I75" s="12"/>
       <c r="J75" s="12"/>
       <c r="K75" s="12"/>
       <c r="L75" s="12"/>
     </row>
-    <row r="76" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="11"/>
-      <c r="B76" s="91"/>
-      <c r="C76" s="94"/>
-      <c r="D76" s="94"/>
-      <c r="E76" s="94"/>
-      <c r="F76" s="94"/>
-      <c r="G76" s="94"/>
+    <row r="76" spans="1:12" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="1"/>
+      <c r="B76" s="39"/>
+      <c r="C76" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="D76" s="48" t="s">
+        <v>57</v>
+      </c>
+      <c r="E76" s="49"/>
+      <c r="F76" s="60" t="s">
+        <v>38</v>
+      </c>
+      <c r="G76" s="49"/>
       <c r="H76" s="12"/>
       <c r="I76" s="12"/>
       <c r="J76" s="12"/>
       <c r="K76" s="12"/>
       <c r="L76" s="12"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="11"/>
-      <c r="B77" s="91"/>
-      <c r="C77" s="94"/>
-      <c r="D77" s="94"/>
-      <c r="E77" s="94"/>
-      <c r="F77" s="94"/>
-      <c r="G77" s="94"/>
+      <c r="B77" s="39"/>
+      <c r="C77" s="40"/>
+      <c r="D77" s="48"/>
+      <c r="E77" s="49"/>
+      <c r="F77" s="60"/>
+      <c r="G77" s="49"/>
       <c r="H77" s="12"/>
       <c r="I77" s="12"/>
       <c r="J77" s="12"/>
       <c r="K77" s="12"/>
       <c r="L77" s="12"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A78" s="2"/>
-      <c r="B78" s="12"/>
-      <c r="C78" s="91"/>
-      <c r="D78" s="91"/>
-      <c r="E78" s="91"/>
-      <c r="F78" s="91"/>
-      <c r="G78" s="91"/>
+    <row r="78" spans="1:12" ht="62.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="11"/>
+      <c r="B78" s="39"/>
+      <c r="C78" s="41"/>
+      <c r="D78" s="48"/>
+      <c r="E78" s="49"/>
+      <c r="F78" s="60"/>
+      <c r="G78" s="49"/>
       <c r="H78" s="12"/>
       <c r="I78" s="12"/>
       <c r="J78" s="12"/>
       <c r="K78" s="12"/>
       <c r="L78" s="12"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A79" s="2"/>
-      <c r="B79" s="12"/>
-      <c r="C79" s="12"/>
-      <c r="D79" s="12"/>
-      <c r="E79" s="12"/>
-      <c r="F79" s="12"/>
-      <c r="G79" s="12"/>
+    <row r="79" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="11"/>
+      <c r="B79" s="39"/>
+      <c r="C79" s="42"/>
+      <c r="D79" s="42"/>
+      <c r="E79" s="42"/>
+      <c r="F79" s="42"/>
+      <c r="G79" s="42"/>
       <c r="H79" s="12"/>
       <c r="I79" s="12"/>
-      <c r="J79" s="12"/>
+      <c r="J79" s="12" t="s">
+        <v>52</v>
+      </c>
       <c r="K79" s="12"/>
       <c r="L79" s="12"/>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A80" s="2"/>
-      <c r="B80" s="12"/>
-      <c r="C80" s="12"/>
-      <c r="D80" s="12"/>
-      <c r="E80" s="12"/>
-      <c r="F80" s="12"/>
-      <c r="G80" s="12"/>
+      <c r="A80" s="11"/>
+      <c r="B80" s="39"/>
+      <c r="C80" s="42"/>
+      <c r="D80" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="E80" s="42"/>
+      <c r="F80" s="42"/>
+      <c r="G80" s="42"/>
       <c r="H80" s="12"/>
       <c r="I80" s="12"/>
       <c r="J80" s="12"/>
@@ -2561,18 +2660,20 @@
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="12"/>
-      <c r="C81" s="12"/>
-      <c r="D81" s="12"/>
-      <c r="E81" s="12"/>
-      <c r="F81" s="12"/>
-      <c r="G81" s="12"/>
+      <c r="C81" s="39"/>
+      <c r="D81" s="39"/>
+      <c r="E81" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="F81" s="39"/>
+      <c r="G81" s="39"/>
       <c r="H81" s="12"/>
       <c r="I81" s="12"/>
       <c r="J81" s="12"/>
       <c r="K81" s="12"/>
       <c r="L81" s="12"/>
     </row>
-    <row r="82" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="12"/>
       <c r="C82" s="12"/>
@@ -2586,115 +2687,158 @@
       <c r="K82" s="12"/>
       <c r="L82" s="12"/>
     </row>
-    <row r="83" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="12"/>
-      <c r="C83" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="D83" s="18"/>
-      <c r="E83" s="18"/>
-      <c r="F83" s="18"/>
-      <c r="G83" s="19"/>
+      <c r="C83" s="12"/>
+      <c r="D83" s="12"/>
+      <c r="E83" s="12"/>
+      <c r="F83" s="12"/>
+      <c r="G83" s="12"/>
       <c r="H83" s="12"/>
       <c r="I83" s="12"/>
       <c r="J83" s="12"/>
       <c r="K83" s="12"/>
       <c r="L83" s="12"/>
     </row>
-    <row r="84" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C84" s="95" t="s">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A84" s="2"/>
+      <c r="B84" s="12"/>
+      <c r="C84" s="12"/>
+      <c r="D84" s="12"/>
+      <c r="E84" s="12"/>
+      <c r="F84" s="12"/>
+      <c r="G84" s="12"/>
+      <c r="H84" s="12"/>
+      <c r="I84" s="12"/>
+      <c r="J84" s="12"/>
+      <c r="K84" s="12"/>
+      <c r="L84" s="12"/>
+    </row>
+    <row r="85" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="2"/>
+      <c r="B85" s="12"/>
+      <c r="C85" s="12"/>
+      <c r="D85" s="12"/>
+      <c r="E85" s="12"/>
+      <c r="F85" s="12"/>
+      <c r="G85" s="12"/>
+      <c r="H85" s="12"/>
+      <c r="I85" s="12"/>
+      <c r="J85" s="12"/>
+      <c r="K85" s="12"/>
+      <c r="L85" s="12"/>
+    </row>
+    <row r="86" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="2"/>
+      <c r="B86" s="12"/>
+      <c r="C86" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="D86" s="55"/>
+      <c r="E86" s="55"/>
+      <c r="F86" s="55"/>
+      <c r="G86" s="56"/>
+      <c r="H86" s="12"/>
+      <c r="I86" s="12"/>
+      <c r="J86" s="12"/>
+      <c r="K86" s="12"/>
+      <c r="L86" s="12"/>
+    </row>
+    <row r="87" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C87" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="D84" s="96" t="s">
+      <c r="D87" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="E84" s="82"/>
-      <c r="F84" s="81" t="s">
-        <v>20</v>
-      </c>
-      <c r="G84" s="82"/>
-    </row>
-    <row r="85" spans="1:12" ht="270.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C85" s="97" t="s">
-        <v>43</v>
-      </c>
-      <c r="D85" s="90"/>
-      <c r="E85" s="85"/>
-      <c r="F85" s="84"/>
-      <c r="G85" s="85"/>
-    </row>
-    <row r="86" spans="1:12" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C86" s="98" t="s">
-        <v>44</v>
-      </c>
-      <c r="D86" s="90"/>
-      <c r="E86" s="85"/>
-      <c r="F86" s="99"/>
-      <c r="G86" s="100"/>
-    </row>
-    <row r="87" spans="1:12" ht="315.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C87" s="101" t="s">
-        <v>45</v>
-      </c>
-      <c r="D87" s="90"/>
-      <c r="E87" s="90"/>
-      <c r="F87" s="102"/>
-      <c r="G87" s="103"/>
+      <c r="E87" s="58"/>
+      <c r="F87" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="G87" s="58"/>
+    </row>
+    <row r="88" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C88" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="D88" s="48"/>
+      <c r="E88" s="49"/>
+      <c r="F88" s="60"/>
+      <c r="G88" s="49"/>
+    </row>
+    <row r="89" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C89" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="D89" s="48"/>
+      <c r="E89" s="49"/>
+      <c r="F89" s="50"/>
+      <c r="G89" s="51"/>
+    </row>
+    <row r="90" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C90" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="D90" s="48"/>
+      <c r="E90" s="48"/>
+      <c r="F90" s="52"/>
+      <c r="G90" s="53"/>
     </row>
   </sheetData>
-  <mergeCells count="51">
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="F86:G86"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="F87:G87"/>
-    <mergeCell ref="C83:G83"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="F84:G84"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="F85:G85"/>
-    <mergeCell ref="F71:G71"/>
+  <mergeCells count="52">
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="F78:G78"/>
+    <mergeCell ref="C69:G69"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="C71:G71"/>
     <mergeCell ref="D72:E72"/>
     <mergeCell ref="F72:G72"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C37:G46"/>
+    <mergeCell ref="C48:G48"/>
+    <mergeCell ref="C49:G49"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="F2:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="F55:G55"/>
     <mergeCell ref="F56:G56"/>
     <mergeCell ref="F57:G57"/>
     <mergeCell ref="F58:G58"/>
     <mergeCell ref="F59:G59"/>
     <mergeCell ref="F60:G60"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="F2:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C37:G46"/>
-    <mergeCell ref="C48:G48"/>
-    <mergeCell ref="C49:G49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="C68:G68"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="F69:G69"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="F70:G70"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="F68:G68"/>
     <mergeCell ref="F74:G74"/>
     <mergeCell ref="D75:E75"/>
     <mergeCell ref="F75:G75"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="F89:G89"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="F90:G90"/>
+    <mergeCell ref="C86:G86"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="F87:G87"/>
+    <mergeCell ref="D88:E88"/>
+    <mergeCell ref="F88:G88"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C5" r:id="rId1" xr:uid="{21D9B59C-823B-4354-BAE2-7BC546DA995A}"/>

</xml_diff>